<commit_message>
subo las correcciones del 28/11
</commit_message>
<xml_diff>
--- a/5_Pasaje_a_Modo_Protegido/solucion/GDT Entradas.xlsx
+++ b/5_Pasaje_a_Modo_Protegido/solucion/GDT Entradas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="57">
   <si>
     <t xml:space="preserve">Un segmento para código de nivel 0 ejecutar/lectura</t>
   </si>
@@ -201,7 +201,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -252,12 +252,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -321,7 +315,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -347,10 +341,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -438,10 +428,10 @@
   <dimension ref="A1:AI37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AL17" activeCellId="0" sqref="AL17"/>
+      <selection pane="topLeft" activeCell="R12" activeCellId="0" sqref="R12:AG12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="1" style="0" width="2.38"/>
   </cols>
@@ -747,24 +737,24 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1"/>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
       <c r="R6" s="6" t="s">
         <v>51</v>
       </c>
@@ -1087,25 +1077,27 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
-      <c r="R12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1425,24 +1417,24 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
-      <c r="K18" s="7"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
       <c r="R18" s="6" t="s">
         <v>51</v>
       </c>
@@ -1765,24 +1757,24 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1"/>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="7"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
       <c r="R24" s="6" t="s">
         <v>51</v>
       </c>
@@ -1806,7 +1798,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1"/>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>56</v>
       </c>
       <c r="C25" s="1"/>

</xml_diff>